<commit_message>
Converted all .xlsx to .csv
Converted all of the datasets into .csv format.
</commit_message>
<xml_diff>
--- a/Development/datasets/Tainan2020dataset.xlsx
+++ b/Development/datasets/Tainan2020dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="95">
   <si>
     <t xml:space="preserve">age_years</t>
   </si>
@@ -55,49 +55,267 @@
     <t xml:space="preserve">tumorProgression_no0_yes1</t>
   </si>
   <si>
-    <t xml:space="preserve">year_of_diagnosis_2005-2010(0)_2010-2016(1)</t>
+    <t xml:space="preserve">year_of_diagnosis_05-10(0)_10-16(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.12</t>
   </si>
   <si>
     <t xml:space="preserve">60.00</t>
   </si>
   <si>
+    <t xml:space="preserve">61.38</t>
+  </si>
+  <si>
     <t xml:space="preserve">66.00</t>
   </si>
   <si>
+    <t xml:space="preserve">7.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.95</t>
+  </si>
+  <si>
     <t xml:space="preserve">59.40</t>
   </si>
   <si>
+    <t xml:space="preserve">6.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54.93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.36</t>
+  </si>
+  <si>
     <t xml:space="preserve">61.20</t>
   </si>
   <si>
+    <t xml:space="preserve">7.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.28</t>
+  </si>
+  <si>
     <t xml:space="preserve">64.80</t>
   </si>
   <si>
+    <t xml:space="preserve">14.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.50</t>
+  </si>
+  <si>
     <t xml:space="preserve">50.00</t>
   </si>
   <si>
+    <t xml:space="preserve">13.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.98</t>
+  </si>
+  <si>
     <t xml:space="preserve">63.00</t>
   </si>
   <si>
+    <t xml:space="preserve">14.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.8</t>
+  </si>
+  <si>
     <t xml:space="preserve">54.00</t>
   </si>
   <si>
+    <t xml:space="preserve">16.43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.65</t>
+  </si>
+  <si>
     <t xml:space="preserve">62.70</t>
   </si>
   <si>
     <t xml:space="preserve">66.60</t>
   </si>
   <si>
+    <t xml:space="preserve">14.26</t>
+  </si>
+  <si>
     <t xml:space="preserve">58.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00_ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00_ "/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -165,7 +383,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,8 +400,16 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -377,8 +603,8 @@
   </sheetPr>
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -386,7 +612,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.94"/>
@@ -397,7 +623,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="38.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="10.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,7 +636,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -448,11 +674,11 @@
       <c r="C2" s="1" t="n">
         <v>16.32</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>15.1232876712329</v>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>731</v>
@@ -475,7 +701,7 @@
       <c r="L2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M2" s="4"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -487,11 +713,11 @@
       <c r="C3" s="1" t="n">
         <v>106.08</v>
       </c>
-      <c r="D3" s="4" t="n">
-        <v>61.3808219178083</v>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0</v>
@@ -511,7 +737,7 @@
       <c r="L3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="4"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -523,11 +749,11 @@
       <c r="C4" s="1" t="n">
         <v>17.52</v>
       </c>
-      <c r="D4" s="4" t="n">
-        <v>7.69315068493151</v>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>215</v>
@@ -550,7 +776,7 @@
       <c r="L4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M4" s="4"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -562,11 +788,11 @@
       <c r="C5" s="1" t="n">
         <v>29.04</v>
       </c>
-      <c r="D5" s="4" t="n">
-        <v>7.82465753424658</v>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>255</v>
@@ -586,7 +812,7 @@
       <c r="L5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -598,11 +824,11 @@
       <c r="C6" s="1" t="n">
         <v>15.12</v>
       </c>
-      <c r="D6" s="4" t="n">
-        <v>12.9534246575342</v>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>154</v>
@@ -625,7 +851,7 @@
       <c r="L6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -637,11 +863,11 @@
       <c r="C7" s="1" t="n">
         <v>10.2</v>
       </c>
-      <c r="D7" s="4" t="n">
-        <v>6.41095890410959</v>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>0</v>
@@ -661,7 +887,7 @@
       <c r="L7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -673,11 +899,11 @@
       <c r="C8" s="1" t="n">
         <v>77.16</v>
       </c>
-      <c r="D8" s="4" t="n">
-        <v>54.9369863013698</v>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>322</v>
@@ -700,7 +926,7 @@
       <c r="L8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -712,11 +938,11 @@
       <c r="C9" s="1" t="n">
         <v>7.56</v>
       </c>
-      <c r="D9" s="4" t="n">
-        <v>4.76712328767124</v>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>166</v>
@@ -739,7 +965,7 @@
       <c r="L9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -751,11 +977,11 @@
       <c r="C10" s="1" t="n">
         <v>11.52</v>
       </c>
-      <c r="D10" s="4" t="n">
-        <v>11.4082191780822</v>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>317</v>
@@ -778,7 +1004,7 @@
       <c r="L10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -790,11 +1016,11 @@
       <c r="C11" s="1" t="n">
         <v>15.84</v>
       </c>
-      <c r="D11" s="4" t="n">
-        <v>13.3808219178083</v>
+      <c r="D11" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>246</v>
@@ -817,7 +1043,7 @@
       <c r="L11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -829,11 +1055,11 @@
       <c r="C12" s="1" t="n">
         <v>33.84</v>
       </c>
-      <c r="D12" s="4" t="n">
-        <v>14.3671232876712</v>
+      <c r="D12" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>247</v>
@@ -856,7 +1082,7 @@
       <c r="L12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -868,11 +1094,11 @@
       <c r="C13" s="1" t="n">
         <v>9.24</v>
       </c>
-      <c r="D13" s="4" t="n">
-        <v>7.06849315068493</v>
+      <c r="D13" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>0</v>
@@ -889,7 +1115,7 @@
       <c r="L13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M13" s="4"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -901,11 +1127,11 @@
       <c r="C14" s="1" t="n">
         <v>10.08</v>
       </c>
-      <c r="D14" s="4" t="n">
-        <v>7.95616438356164</v>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>141</v>
@@ -928,7 +1154,7 @@
       <c r="L14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M14" s="4"/>
+      <c r="M14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -940,11 +1166,11 @@
       <c r="C15" s="1" t="n">
         <v>28.56</v>
       </c>
-      <c r="D15" s="4" t="n">
-        <v>5.58904109589041</v>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>473</v>
@@ -967,7 +1193,7 @@
       <c r="L15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M15" s="4"/>
+      <c r="M15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -979,11 +1205,11 @@
       <c r="C16" s="1" t="n">
         <v>2.76</v>
       </c>
-      <c r="D16" s="4" t="n">
-        <v>2.72876712328768</v>
+      <c r="D16" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>251</v>
@@ -1003,7 +1229,7 @@
       <c r="L16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M16" s="4"/>
+      <c r="M16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1015,11 +1241,11 @@
       <c r="C17" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="D17" s="4" t="n">
-        <v>9.36986301369863</v>
+      <c r="D17" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G17" s="1" t="n">
         <v>0</v>
@@ -1036,7 +1262,7 @@
       <c r="L17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M17" s="4"/>
+      <c r="M17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1052,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G18" s="1" t="n">
         <v>0</v>
@@ -1069,7 +1295,7 @@
       <c r="L18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M18" s="4"/>
+      <c r="M18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1081,11 +1307,11 @@
       <c r="C19" s="1" t="n">
         <v>14.16</v>
       </c>
-      <c r="D19" s="4" t="n">
-        <v>5.98356164383561</v>
+      <c r="D19" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G19" s="1" t="n">
         <v>1</v>
@@ -1105,7 +1331,7 @@
       <c r="L19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M19" s="4"/>
+      <c r="M19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -1117,11 +1343,11 @@
       <c r="C20" s="1" t="n">
         <v>64.8</v>
       </c>
-      <c r="D20" s="4" t="n">
-        <v>13.2821917808219</v>
+      <c r="D20" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G20" s="1" t="n">
         <v>1</v>
@@ -1138,7 +1364,7 @@
       <c r="L20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M20" s="4"/>
+      <c r="M20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -1150,11 +1376,11 @@
       <c r="C21" s="1" t="n">
         <v>23.16</v>
       </c>
-      <c r="D21" s="4" t="n">
-        <v>14.7945205479452</v>
+      <c r="D21" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>124</v>
@@ -1177,7 +1403,7 @@
       <c r="L21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M21" s="4"/>
+      <c r="M21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -1189,11 +1415,11 @@
       <c r="C22" s="1" t="n">
         <v>7.08</v>
       </c>
-      <c r="D22" s="4" t="n">
-        <v>5.19452054794521</v>
+      <c r="D22" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>339</v>
@@ -1216,7 +1442,7 @@
       <c r="L22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M22" s="4"/>
+      <c r="M22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -1228,11 +1454,11 @@
       <c r="C23" s="1" t="n">
         <v>5.76</v>
       </c>
-      <c r="D23" s="4" t="n">
-        <v>3.68219178082192</v>
+      <c r="D23" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>239</v>
@@ -1255,7 +1481,7 @@
       <c r="L23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M23" s="4"/>
+      <c r="M23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -1267,11 +1493,11 @@
       <c r="C24" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="D24" s="4" t="n">
-        <v>16.6684931506849</v>
+      <c r="D24" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>287</v>
@@ -1291,7 +1517,7 @@
       <c r="L24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M24" s="4"/>
+      <c r="M24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -1303,11 +1529,11 @@
       <c r="C25" s="1" t="n">
         <v>16.08</v>
       </c>
-      <c r="D25" s="4" t="n">
-        <v>8.97534246575343</v>
+      <c r="D25" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F25" s="1" t="n">
         <v>664</v>
@@ -1327,7 +1553,7 @@
       <c r="L25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M25" s="4"/>
+      <c r="M25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1339,11 +1565,11 @@
       <c r="C26" s="1" t="n">
         <v>10.8</v>
       </c>
-      <c r="D26" s="4" t="n">
-        <v>5.78630136986302</v>
+      <c r="D26" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>310</v>
@@ -1363,7 +1589,7 @@
       <c r="L26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M26" s="4"/>
+      <c r="M26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -1375,11 +1601,11 @@
       <c r="C27" s="1" t="n">
         <v>13.44</v>
       </c>
-      <c r="D27" s="4" t="n">
-        <v>6.70684931506849</v>
+      <c r="D27" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>244</v>
@@ -1402,7 +1628,7 @@
       <c r="L27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M27" s="4"/>
+      <c r="M27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -1414,11 +1640,11 @@
       <c r="C28" s="1" t="n">
         <v>6.96</v>
       </c>
-      <c r="D28" s="4" t="n">
-        <v>6.9041095890411</v>
+      <c r="D28" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G28" s="1" t="n">
         <v>0</v>
@@ -1438,7 +1664,7 @@
       <c r="L28" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M28" s="4"/>
+      <c r="M28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -1450,11 +1676,11 @@
       <c r="C29" s="1" t="n">
         <v>12.12</v>
       </c>
-      <c r="D29" s="4" t="n">
-        <v>13.0520547945205</v>
+      <c r="D29" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>173</v>
@@ -1474,7 +1700,7 @@
       <c r="L29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M29" s="4"/>
+      <c r="M29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -1486,11 +1712,11 @@
       <c r="C30" s="1" t="n">
         <v>10.56</v>
       </c>
-      <c r="D30" s="4" t="n">
-        <v>3.41917808219178</v>
+      <c r="D30" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>242</v>
@@ -1510,7 +1736,7 @@
       <c r="L30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M30" s="4"/>
+      <c r="M30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -1522,11 +1748,11 @@
       <c r="C31" s="1" t="n">
         <v>7.44</v>
       </c>
-      <c r="D31" s="4" t="n">
-        <v>3.64931506849315</v>
+      <c r="D31" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F31" s="1" t="n">
         <v>208</v>
@@ -1549,7 +1775,7 @@
       <c r="L31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M31" s="4"/>
+      <c r="M31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
@@ -1561,11 +1787,11 @@
       <c r="C32" s="1" t="n">
         <v>19.08</v>
       </c>
-      <c r="D32" s="4" t="n">
-        <v>14.7287671232876</v>
+      <c r="D32" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>341</v>
@@ -1585,7 +1811,7 @@
       <c r="L32" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M32" s="4"/>
+      <c r="M32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -1597,11 +1823,11 @@
       <c r="C33" s="1" t="n">
         <v>27.96</v>
       </c>
-      <c r="D33" s="4" t="n">
-        <v>20.7780821917808</v>
+      <c r="D33" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>1</v>
@@ -1618,7 +1844,7 @@
       <c r="L33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M33" s="4"/>
+      <c r="M33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
@@ -1630,11 +1856,11 @@
       <c r="C34" s="1" t="n">
         <v>19.92</v>
       </c>
-      <c r="D34" s="4" t="n">
-        <v>9.23835616438356</v>
+      <c r="D34" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F34" s="1" t="n">
         <v>173</v>
@@ -1657,7 +1883,7 @@
       <c r="L34" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M34" s="4"/>
+      <c r="M34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -1669,11 +1895,11 @@
       <c r="C35" s="1" t="n">
         <v>13.32</v>
       </c>
-      <c r="D35" s="4" t="n">
-        <v>5.45753424657534</v>
+      <c r="D35" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>150</v>
@@ -1693,7 +1919,7 @@
       <c r="L35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M35" s="4"/>
+      <c r="M35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -1705,11 +1931,11 @@
       <c r="C36" s="1" t="n">
         <v>9.48</v>
       </c>
-      <c r="D36" s="4" t="n">
-        <v>9.5013698630137</v>
+      <c r="D36" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F36" s="1" t="n">
         <v>623</v>
@@ -1732,7 +1958,7 @@
       <c r="L36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M36" s="4"/>
+      <c r="M36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -1744,11 +1970,11 @@
       <c r="C37" s="1" t="n">
         <v>13.32</v>
       </c>
-      <c r="D37" s="4" t="n">
-        <v>13.3150684931507</v>
+      <c r="D37" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F37" s="1" t="n">
         <v>512</v>
@@ -1768,7 +1994,7 @@
       <c r="L37" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M37" s="4"/>
+      <c r="M37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
@@ -1780,11 +2006,11 @@
       <c r="C38" s="1" t="n">
         <v>35.04</v>
       </c>
-      <c r="D38" s="4" t="n">
-        <v>34.9808219178083</v>
+      <c r="D38" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>1</v>
@@ -1804,7 +2030,7 @@
       <c r="L38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M38" s="4"/>
+      <c r="M38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -1816,11 +2042,11 @@
       <c r="C39" s="1" t="n">
         <v>14.64</v>
       </c>
-      <c r="D39" s="4" t="n">
-        <v>14.695890410959</v>
+      <c r="D39" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F39" s="1" t="n">
         <v>56</v>
@@ -1843,7 +2069,7 @@
       <c r="L39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M39" s="4"/>
+      <c r="M39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -1855,11 +2081,11 @@
       <c r="C40" s="1" t="n">
         <v>22.8</v>
       </c>
-      <c r="D40" s="4" t="n">
-        <v>16.0767123287671</v>
+      <c r="D40" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>0</v>
@@ -1876,7 +2102,7 @@
       <c r="L40" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M40" s="4"/>
+      <c r="M40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
@@ -1888,11 +2114,11 @@
       <c r="C41" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D41" s="4" t="n">
-        <v>26.958904109589</v>
+      <c r="D41" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F41" s="1" t="n">
         <v>205</v>
@@ -1915,7 +2141,7 @@
       <c r="L41" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M41" s="4"/>
+      <c r="M41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -1927,11 +2153,11 @@
       <c r="C42" s="1" t="n">
         <v>3.84</v>
       </c>
-      <c r="D42" s="4" t="n">
-        <v>3.64931506849315</v>
+      <c r="D42" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F42" s="1" t="n">
         <v>649</v>
@@ -1954,7 +2180,7 @@
       <c r="L42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M42" s="4"/>
+      <c r="M42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -1966,11 +2192,11 @@
       <c r="C43" s="1" t="n">
         <v>26.64</v>
       </c>
-      <c r="D43" s="4" t="n">
-        <v>18.5424657534246</v>
+      <c r="D43" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F43" s="1" t="n">
         <v>228</v>
@@ -1993,7 +2219,7 @@
       <c r="L43" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M43" s="4"/>
+      <c r="M43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
@@ -2005,11 +2231,11 @@
       <c r="C44" s="1" t="n">
         <v>109.8</v>
       </c>
-      <c r="D44" s="4" t="n">
-        <v>16.8</v>
+      <c r="D44" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F44" s="1" t="n">
         <v>817</v>
@@ -2032,7 +2258,7 @@
       <c r="L44" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M44" s="4"/>
+      <c r="M44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -2048,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="F45" s="1" t="n">
         <v>183</v>
@@ -2071,7 +2297,7 @@
       <c r="L45" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M45" s="4"/>
+      <c r="M45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
@@ -2083,11 +2309,11 @@
       <c r="C46" s="1" t="n">
         <v>16.44</v>
       </c>
-      <c r="D46" s="4" t="n">
-        <v>16.4383561643836</v>
+      <c r="D46" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F46" s="1" t="n">
         <v>261</v>
@@ -2110,7 +2336,7 @@
       <c r="L46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M46" s="4"/>
+      <c r="M46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
@@ -2122,11 +2348,11 @@
       <c r="C47" s="1" t="n">
         <v>41.4</v>
       </c>
-      <c r="D47" s="4" t="n">
-        <v>22.0931506849315</v>
+      <c r="D47" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F47" s="1" t="n">
         <v>100</v>
@@ -2149,7 +2375,7 @@
       <c r="L47" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M47" s="4"/>
+      <c r="M47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -2161,11 +2387,11 @@
       <c r="C48" s="1" t="n">
         <v>60.84</v>
       </c>
-      <c r="D48" s="4" t="n">
-        <v>6.8054794520548</v>
+      <c r="D48" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F48" s="1" t="n">
         <v>395</v>
@@ -2188,7 +2414,7 @@
       <c r="L48" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M48" s="4"/>
+      <c r="M48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
@@ -2200,11 +2426,11 @@
       <c r="C49" s="1" t="n">
         <v>21.84</v>
       </c>
-      <c r="D49" s="4" t="n">
-        <v>8.94246575342466</v>
+      <c r="D49" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F49" s="1" t="n">
         <v>142</v>
@@ -2227,7 +2453,7 @@
       <c r="L49" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M49" s="4"/>
+      <c r="M49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
@@ -2239,11 +2465,11 @@
       <c r="C50" s="1" t="n">
         <v>4.92</v>
       </c>
-      <c r="D50" s="4" t="n">
-        <v>4.8986301369863</v>
+      <c r="D50" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F50" s="1" t="n">
         <v>600</v>
@@ -2263,7 +2489,7 @@
       <c r="L50" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M50" s="4"/>
+      <c r="M50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
@@ -2275,11 +2501,11 @@
       <c r="C51" s="1" t="n">
         <v>11.4</v>
       </c>
-      <c r="D51" s="4" t="n">
-        <v>10.6191780821918</v>
+      <c r="D51" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F51" s="1" t="n">
         <v>325</v>
@@ -2299,7 +2525,7 @@
       <c r="L51" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M51" s="4"/>
+      <c r="M51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
@@ -2311,11 +2537,11 @@
       <c r="C52" s="1" t="n">
         <v>11.76</v>
       </c>
-      <c r="D52" s="4" t="n">
-        <v>9.63287671232876</v>
+      <c r="D52" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F52" s="1" t="n">
         <v>154</v>
@@ -2338,7 +2564,7 @@
       <c r="L52" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M52" s="4"/>
+      <c r="M52" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
@@ -2350,11 +2576,11 @@
       <c r="C53" s="1" t="n">
         <v>16.56</v>
       </c>
-      <c r="D53" s="4" t="n">
-        <v>16.504109589041</v>
+      <c r="D53" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F53" s="1" t="n">
         <v>94</v>
@@ -2377,7 +2603,7 @@
       <c r="L53" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M53" s="4"/>
+      <c r="M53" s="5"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
@@ -2389,11 +2615,11 @@
       <c r="C54" s="1" t="n">
         <v>21.84</v>
       </c>
-      <c r="D54" s="4" t="n">
-        <v>12.7232876712329</v>
+      <c r="D54" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F54" s="1" t="n">
         <v>214</v>
@@ -2416,7 +2642,7 @@
       <c r="L54" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M54" s="4"/>
+      <c r="M54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
@@ -2428,11 +2654,11 @@
       <c r="C55" s="1" t="n">
         <v>32.16</v>
       </c>
-      <c r="D55" s="4" t="n">
-        <v>23.8356164383561</v>
+      <c r="D55" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G55" s="1" t="n">
         <v>1</v>
@@ -2452,7 +2678,7 @@
       <c r="L55" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M55" s="4"/>
+      <c r="M55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
@@ -2464,11 +2690,11 @@
       <c r="C56" s="1" t="n">
         <v>10.68</v>
       </c>
-      <c r="D56" s="4" t="n">
-        <v>6.31232876712329</v>
+      <c r="D56" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F56" s="1" t="n">
         <v>324</v>
@@ -2491,7 +2717,7 @@
       <c r="L56" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M56" s="4"/>
+      <c r="M56" s="5"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
@@ -2503,11 +2729,11 @@
       <c r="C57" s="1" t="n">
         <v>20.16</v>
       </c>
-      <c r="D57" s="4" t="n">
-        <v>9.10684931506849</v>
+      <c r="D57" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G57" s="1" t="n">
         <v>1</v>
@@ -2527,7 +2753,7 @@
       <c r="L57" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M57" s="4"/>
+      <c r="M57" s="5"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
@@ -2539,11 +2765,11 @@
       <c r="C58" s="1" t="n">
         <v>21.24</v>
       </c>
-      <c r="D58" s="4" t="n">
-        <v>18.4109589041096</v>
+      <c r="D58" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G58" s="1" t="n">
         <v>0</v>
@@ -2563,7 +2789,7 @@
       <c r="L58" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M58" s="4"/>
+      <c r="M58" s="5"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
@@ -2575,11 +2801,11 @@
       <c r="C59" s="1" t="n">
         <v>20.04</v>
       </c>
-      <c r="D59" s="4" t="n">
-        <v>17.4575342465754</v>
+      <c r="D59" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F59" s="1" t="n">
         <v>334</v>
@@ -2602,7 +2828,7 @@
       <c r="L59" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M59" s="4"/>
+      <c r="M59" s="5"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
@@ -2614,11 +2840,11 @@
       <c r="C60" s="1" t="n">
         <v>4.2</v>
       </c>
-      <c r="D60" s="4" t="n">
-        <v>4.04383561643836</v>
+      <c r="D60" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F60" s="1" t="n">
         <v>456</v>
@@ -2641,7 +2867,7 @@
       <c r="L60" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M60" s="4"/>
+      <c r="M60" s="5"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
@@ -2653,11 +2879,11 @@
       <c r="C61" s="1" t="n">
         <v>20.52</v>
       </c>
-      <c r="D61" s="4" t="n">
-        <v>7.06849315068493</v>
+      <c r="D61" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F61" s="1" t="n">
         <v>125</v>
@@ -2680,7 +2906,7 @@
       <c r="L61" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M61" s="4"/>
+      <c r="M61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
@@ -2692,11 +2918,11 @@
       <c r="C62" s="1" t="n">
         <v>10.8</v>
       </c>
-      <c r="D62" s="4" t="n">
-        <v>2.99178082191781</v>
+      <c r="D62" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F62" s="1" t="n">
         <v>367</v>
@@ -2719,7 +2945,7 @@
       <c r="L62" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M62" s="4"/>
+      <c r="M62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
@@ -2731,11 +2957,11 @@
       <c r="C63" s="1" t="n">
         <v>8.76</v>
       </c>
-      <c r="D63" s="4" t="n">
-        <v>5.78630136986302</v>
+      <c r="D63" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F63" s="1" t="n">
         <v>239</v>
@@ -2758,7 +2984,7 @@
       <c r="L63" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M63" s="4"/>
+      <c r="M63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
@@ -2770,11 +2996,11 @@
       <c r="C64" s="1" t="n">
         <v>6.36</v>
       </c>
-      <c r="D64" s="4" t="n">
-        <v>6.31232876712329</v>
+      <c r="D64" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F64" s="1" t="n">
         <v>141</v>
@@ -2797,7 +3023,7 @@
       <c r="L64" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M64" s="4"/>
+      <c r="M64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
@@ -2809,11 +3035,11 @@
       <c r="C65" s="1" t="n">
         <v>8.16</v>
       </c>
-      <c r="D65" s="4" t="n">
-        <v>8.12054794520548</v>
+      <c r="D65" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G65" s="1" t="n">
         <v>0</v>
@@ -2833,7 +3059,7 @@
       <c r="L65" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M65" s="4"/>
+      <c r="M65" s="5"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
@@ -2845,11 +3071,11 @@
       <c r="C66" s="1" t="n">
         <v>12.48</v>
       </c>
-      <c r="D66" s="4" t="n">
-        <v>8.31780821917808</v>
+      <c r="D66" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G66" s="1" t="n">
         <v>0</v>
@@ -2869,7 +3095,7 @@
       <c r="L66" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M66" s="4"/>
+      <c r="M66" s="5"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
@@ -2881,11 +3107,11 @@
       <c r="C67" s="1" t="n">
         <v>24.6</v>
       </c>
-      <c r="D67" s="4" t="n">
-        <v>24.7561643835617</v>
+      <c r="D67" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F67" s="1" t="n">
         <v>283</v>
@@ -2908,7 +3134,7 @@
       <c r="L67" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M67" s="4"/>
+      <c r="M67" s="5"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
@@ -2920,11 +3146,11 @@
       <c r="C68" s="1" t="n">
         <v>10.56</v>
       </c>
-      <c r="D68" s="4" t="n">
-        <v>3.74794520547946</v>
+      <c r="D68" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F68" s="1" t="n">
         <v>327</v>
@@ -2947,7 +3173,7 @@
       <c r="L68" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M68" s="4"/>
+      <c r="M68" s="5"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
@@ -2959,11 +3185,11 @@
       <c r="C69" s="1" t="n">
         <v>17.16</v>
       </c>
-      <c r="D69" s="4" t="n">
-        <v>12.6904109589041</v>
+      <c r="D69" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F69" s="1" t="n">
         <v>330</v>
@@ -2986,7 +3212,7 @@
       <c r="L69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M69" s="4"/>
+      <c r="M69" s="5"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
@@ -2998,11 +3224,11 @@
       <c r="C70" s="1" t="n">
         <v>13.8</v>
       </c>
-      <c r="D70" s="4" t="n">
-        <v>6.87123287671233</v>
+      <c r="D70" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F70" s="1" t="n">
         <v>109</v>
@@ -3025,7 +3251,7 @@
       <c r="L70" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M70" s="4"/>
+      <c r="M70" s="5"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
@@ -3041,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G71" s="1" t="n">
         <v>1</v>
@@ -3061,7 +3287,7 @@
       <c r="L71" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M71" s="4"/>
+      <c r="M71" s="5"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
@@ -3073,11 +3299,11 @@
       <c r="C72" s="1" t="n">
         <v>2.52</v>
       </c>
-      <c r="D72" s="4" t="n">
-        <v>2.56438356164383</v>
+      <c r="D72" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="G72" s="1" t="n">
         <v>0</v>
@@ -3097,7 +3323,7 @@
       <c r="L72" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M72" s="4"/>
+      <c r="M72" s="5"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
@@ -3109,11 +3335,11 @@
       <c r="C73" s="1" t="n">
         <v>6.24</v>
       </c>
-      <c r="D73" s="4" t="n">
-        <v>6.27945205479452</v>
+      <c r="D73" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G73" s="1" t="n">
         <v>1</v>
@@ -3133,7 +3359,7 @@
       <c r="L73" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M73" s="4"/>
+      <c r="M73" s="5"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
@@ -3145,11 +3371,11 @@
       <c r="C74" s="1" t="n">
         <v>35.16</v>
       </c>
-      <c r="D74" s="4" t="n">
-        <v>12.558904109589</v>
+      <c r="D74" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G74" s="1" t="n">
         <v>0</v>
@@ -3169,7 +3395,7 @@
       <c r="L74" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M74" s="4"/>
+      <c r="M74" s="5"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
@@ -3181,11 +3407,11 @@
       <c r="C75" s="1" t="n">
         <v>10.92</v>
       </c>
-      <c r="D75" s="4" t="n">
-        <v>5.32602739726027</v>
+      <c r="D75" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G75" s="1" t="n">
         <v>0</v>
@@ -3202,7 +3428,7 @@
       <c r="L75" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M75" s="4"/>
+      <c r="M75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
@@ -3214,11 +3440,11 @@
       <c r="C76" s="1" t="n">
         <v>4.92</v>
       </c>
-      <c r="D76" s="4" t="n">
-        <v>4.93150684931507</v>
+      <c r="D76" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="G76" s="1" t="n">
         <v>0</v>
@@ -3238,7 +3464,7 @@
       <c r="L76" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M76" s="4"/>
+      <c r="M76" s="5"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
@@ -3250,11 +3476,11 @@
       <c r="C77" s="1" t="n">
         <v>12.12</v>
       </c>
-      <c r="D77" s="4" t="n">
-        <v>6.87123287671233</v>
+      <c r="D77" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G77" s="1" t="n">
         <v>1</v>
@@ -3274,7 +3500,7 @@
       <c r="L77" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M77" s="4"/>
+      <c r="M77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
@@ -3290,7 +3516,7 @@
         <v>0</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G78" s="1" t="n">
         <v>1</v>
@@ -3310,7 +3536,7 @@
       <c r="L78" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M78" s="4"/>
+      <c r="M78" s="5"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
@@ -3322,11 +3548,11 @@
       <c r="C79" s="1" t="n">
         <v>5.64</v>
       </c>
-      <c r="D79" s="4" t="n">
-        <v>5.65479452054795</v>
+      <c r="D79" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G79" s="1" t="n">
         <v>1</v>
@@ -3346,7 +3572,7 @@
       <c r="L79" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M79" s="4"/>
+      <c r="M79" s="5"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
@@ -3358,11 +3584,11 @@
       <c r="C80" s="1" t="n">
         <v>13.32</v>
       </c>
-      <c r="D80" s="4" t="n">
-        <v>13.2821917808219</v>
+      <c r="D80" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="G80" s="1" t="n">
         <v>1</v>
@@ -3382,7 +3608,7 @@
       <c r="L80" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M80" s="4"/>
+      <c r="M80" s="5"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
@@ -3398,7 +3624,7 @@
         <v>0</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="G81" s="1" t="n">
         <v>0</v>
@@ -3418,7 +3644,7 @@
       <c r="L81" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M81" s="4"/>
+      <c r="M81" s="5"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
@@ -3430,11 +3656,11 @@
       <c r="C82" s="1" t="n">
         <v>14.28</v>
       </c>
-      <c r="D82" s="4" t="n">
-        <v>14.2684931506849</v>
+      <c r="D82" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="F82" s="1" t="n">
         <v>476</v>
@@ -3457,7 +3683,7 @@
       <c r="L82" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M82" s="4"/>
+      <c r="M82" s="5"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
@@ -3469,11 +3695,11 @@
       <c r="C83" s="1" t="n">
         <v>11.52</v>
       </c>
-      <c r="D83" s="4" t="n">
-        <v>4.27397260273973</v>
+      <c r="D83" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F83" s="1" t="n">
         <v>148</v>
@@ -3493,7 +3719,7 @@
       <c r="L83" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M83" s="4"/>
+      <c r="M83" s="5"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
@@ -3505,11 +3731,11 @@
       <c r="C84" s="1" t="n">
         <v>6.72</v>
       </c>
-      <c r="D84" s="4" t="n">
-        <v>6.70684931506849</v>
+      <c r="D84" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="F84" s="1" t="n">
         <v>714</v>
@@ -3532,7 +3758,7 @@
       <c r="L84" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M84" s="4"/>
+      <c r="M84" s="5"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
@@ -3544,11 +3770,11 @@
       <c r="C85" s="1" t="n">
         <v>3.12</v>
       </c>
-      <c r="D85" s="4" t="n">
-        <v>3.12328767123288</v>
+      <c r="D85" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F85" s="1" t="n">
         <v>203</v>
@@ -3568,7 +3794,7 @@
       <c r="L85" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M85" s="4"/>
+      <c r="M85" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>